<commit_message>
feat: Update translations TB aggregate
</commit_message>
<xml_diff>
--- a/metadata/TB/TB_COMPLETE_V1_DHIS2.33/reference.xlsx
+++ b/metadata/TB/TB_COMPLETE_V1_DHIS2.33/reference.xlsx
@@ -495,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-02-08T15:03</v>
+        <v>2021-02-08T17:28</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>TB_COMPLETE_V1.1.1_DHIS2.33_2021-02-08T15:03</v>
+        <v>TB_COMPLETE_V1.1.1_DHIS2.33_2021-02-08T17:28</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2271,7 @@
         <v>Standard: TB treatment outcomes - second line</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>TB treatment outcome - XDR-TB cases</v>
+        <v>TB treatment outcome - HIV positive RR-TB/MDR-TB cases registered vs all RR-TB/MDR-TB cases registered</v>
       </c>
     </row>
     <row r="3">
@@ -2279,7 +2279,7 @@
         <v>Standard: TB treatment outcomes - second line</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>TB treatment outcome - HIV positive RR-/MDR-TB cases</v>
+        <v>TB treatment outcome - HIV positive RR-TB/MDR-TB cases evaluated vs all RR-TB/MDR-TB cases evaluated</v>
       </c>
     </row>
     <row r="4">
@@ -2287,7 +2287,7 @@
         <v>Standard: TB treatment outcomes - second line</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>TB treatment outcome - HIV positive RR-TB/MDR-TB cases registered vs all RR-TB/MDR-TB cases registered</v>
+        <v>TB treatment outcome - XDR-TB cases</v>
       </c>
     </row>
     <row r="5">
@@ -2295,7 +2295,7 @@
         <v>Standard: TB treatment outcomes - second line</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TB treatment outcome - HIV positive RR-TB/MDR-TB cases evaluated vs all RR-TB/MDR-TB cases evaluated</v>
+        <v>TB treatment outcome - HIV positive RR-/MDR-TB cases</v>
       </c>
     </row>
     <row r="6">
@@ -2311,7 +2311,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>TB - DS-TB drugs redistributed&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
+        <v>TB - GenExpert Cartridges discarded&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
       </c>
     </row>
     <row r="8">
@@ -2319,7 +2319,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>TB - DR-TB drugs discarded&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
+        <v>TB - GenExpert Cartridges distributed&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
       </c>
     </row>
     <row r="9">
@@ -2327,7 +2327,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>TB - DR-TB drugs redistributed&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
+        <v>TB - GenExpert Cartridges redistributed&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
       </c>
     </row>
     <row r="10">
@@ -2335,7 +2335,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>TB - DR-TB drugs stock on hand&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
+        <v>TB - DR-TB drugs distributed&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
       </c>
     </row>
     <row r="11">
@@ -2343,7 +2343,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>TB - DS-TB drugs discarded&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
+        <v>TB - DS-TB drugs redistributed&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
       </c>
     </row>
     <row r="12">
@@ -2351,7 +2351,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>TB - GenExpert Cartridges discarded&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
+        <v>TB - DR-TB drugs discarded&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
       </c>
     </row>
     <row r="13">
@@ -2359,7 +2359,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>TB - GenExpert Cartridges distributed&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
+        <v>TB - DS-TB drugs distributed&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
       </c>
     </row>
     <row r="14">
@@ -2367,7 +2367,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>TB - GenExpert Cartridges redistributed&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
+        <v>TB - DR-TB drugs redistributed&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
       </c>
     </row>
     <row r="15">
@@ -2375,7 +2375,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>TB - DR-TB drugs distributed&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
+        <v>TB - GenExpert Cartridges stock on hand&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
       </c>
     </row>
     <row r="16">
@@ -2383,7 +2383,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>TB - DS-TB drugs distributed&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
+        <v>TB - DR-TB drugs stock on hand&lt;=DR-TB drugs opening balance + DR-TB drugs received</v>
       </c>
     </row>
     <row r="17">
@@ -2391,7 +2391,7 @@
         <v>TB Stock Report</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>TB - GenExpert Cartridges stock on hand&lt;=GenExpert Cartridges opening balance + GenExpert Cartridges received</v>
+        <v>TB - DS-TB drugs discarded&lt;=DS-TB drugs opening balance + DS-TB drugs received</v>
       </c>
     </row>
     <row r="18">
@@ -2575,7 +2575,7 @@
         <v>Standard: Case registration</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>HIV-positive TB patients on co-trimoxazole preventive therapy (CPT)</v>
+        <v>New and relapse TB cases</v>
       </c>
     </row>
     <row r="41">
@@ -2583,7 +2583,7 @@
         <v>Standard: Case registration</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>Bacteriological examinations (TB)</v>
+        <v>HIV-positive TB patients on co-trimoxazole preventive therapy (CPT)</v>
       </c>
     </row>
     <row r="42">
@@ -2591,7 +2591,7 @@
         <v>Standard: Case registration</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>New and relapse TB cases</v>
+        <v>Bacteriological examinations (TB)</v>
       </c>
     </row>
   </sheetData>
@@ -3190,7 +3190,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J11" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -3222,7 +3222,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J12" s="4" t="str">
         <v>pMaektY4E9s</v>
@@ -3446,7 +3446,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I19" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J19" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -3478,7 +3478,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I20" s="4" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J20" s="4" t="str">
         <v>pMaektY4E9s</v>
@@ -3542,7 +3542,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I22" s="4" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J22" s="4" t="str">
         <v>pMaektY4E9s</v>
@@ -3574,7 +3574,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I23" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J23" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -4257,7 +4257,7 @@
         <v>j6wYomVhfNs</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v xml:space="preserve">TB - Laboratory-confirmed MDR-TB cases </v>
+        <v>TB - Laboratory-confirmed MDR-TB cases</v>
       </c>
       <c r="C45" s="5" t="str">
         <v>Lab-confirmed MDR-TB</v>
@@ -4289,10 +4289,10 @@
         <v>J7ChdEuwMPW</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v xml:space="preserve">TB - TB cases tested for HIV or with known HIV status </v>
+        <v>TB - TB cases tested for HIV or with known HIV status</v>
       </c>
       <c r="C46" s="4" t="str">
-        <v xml:space="preserve">TB/HIV tested </v>
+        <v>TB/HIV tested</v>
       </c>
       <c r="D46" s="4" t="str">
         <v>TB_C_HIV_TEST</v>
@@ -4470,7 +4470,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I51" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J51" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -4534,7 +4534,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I53" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J53" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -4609,10 +4609,10 @@
         <v>lRAKLRVIMgp</v>
       </c>
       <c r="B56" s="4" t="str">
-        <v xml:space="preserve">TB - Notified TB cases (all cases, all forms) </v>
+        <v>TB - Notified TB cases (all cases, all forms)</v>
       </c>
       <c r="C56" s="4" t="str">
-        <v xml:space="preserve">All cases (all forms TB) </v>
+        <v>All cases (all forms TB)</v>
       </c>
       <c r="D56" s="4" t="str">
         <v>TB_C_NOTIFIED</v>
@@ -4726,7 +4726,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I59" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J59" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -4769,10 +4769,10 @@
         <v>mPz2CV8PamC</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v xml:space="preserve">TB - TB cases tested for susceptibility to rifampicin </v>
+        <v>TB - TB cases tested for susceptibility to rifampicin</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v xml:space="preserve">Tested for RR-TB </v>
+        <v>Tested for RR-TB</v>
       </c>
       <c r="D61" s="5" t="str">
         <v>TB_C_DST</v>
@@ -5334,7 +5334,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I78" s="4" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J78" s="4" t="str">
         <v>pMaektY4E9s</v>
@@ -5526,7 +5526,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>pMaektY4E9s</v>
@@ -6518,7 +6518,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I115" s="5" t="str">
-        <v>2020-12-17</v>
+        <v>2021-02-08</v>
       </c>
       <c r="J115" s="5" t="str">
         <v>pMaektY4E9s</v>
@@ -10080,7 +10080,7 @@
         <v>Compare subunits using the same graph/Comparez les sous-unités utilisant le même graphique</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2019-08-27</v>
+        <v>2021-02-08</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>BuTAAbV4zMg</v>

</xml_diff>